<commit_message>
Adaptation of input file to flatten the data
</commit_message>
<xml_diff>
--- a/journaux de bord.xlsx
+++ b/journaux de bord.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IA ORA NA" sheetId="4" r:id="rId1"/>
@@ -2339,7 +2339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="778">
   <si>
     <t>Dives-Ouistreham</t>
   </si>
@@ -3110,9 +3110,6 @@
   </si>
   <si>
     <t>Barres-Cedeira</t>
-  </si>
-  <si>
-    <t>auût 97</t>
   </si>
   <si>
     <t>Elantchove-Guetaria</t>
@@ -5159,8 +5156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5231,21 +5228,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="19" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
@@ -5262,16 +5259,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
@@ -5294,7 +5291,7 @@
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19" t="s">
@@ -5322,16 +5319,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -5357,18 +5354,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -5390,18 +5387,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19" t="s">
@@ -5425,25 +5422,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
@@ -5464,7 +5461,7 @@
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>145</v>
@@ -5474,7 +5471,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -5495,11 +5492,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>145</v>
@@ -5509,7 +5506,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -5528,20 +5525,20 @@
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="3"/>
@@ -5567,13 +5564,13 @@
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
@@ -5596,7 +5593,7 @@
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>162</v>
@@ -5604,10 +5601,10 @@
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="3"/>
@@ -5629,18 +5626,18 @@
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J14" s="19"/>
       <c r="K14" s="3"/>
@@ -5660,7 +5657,7 @@
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>1</v>
@@ -5691,7 +5688,7 @@
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>1</v>
@@ -5702,7 +5699,7 @@
         <v>73</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J16" s="19"/>
       <c r="K16" s="3" t="s">
@@ -5722,16 +5719,16 @@
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J17" s="21" t="s">
         <v>39</v>
@@ -5754,19 +5751,19 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
       <c r="H18" s="19" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J18" s="21" t="s">
         <v>40</v>
@@ -5789,19 +5786,19 @@
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="3" t="s">
@@ -5825,16 +5822,16 @@
         <v>4</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="3"/>
@@ -5880,7 +5877,7 @@
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
@@ -5909,16 +5906,16 @@
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
@@ -5940,17 +5937,17 @@
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J24" s="19"/>
       <c r="K24" s="3"/>
@@ -5974,10 +5971,10 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="H25" s="19" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="J25" s="19"/>
       <c r="K25" s="3" t="s">
@@ -6002,21 +5999,21 @@
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
         <v>155</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="J26" s="19"/>
       <c r="K26" s="3" t="s">
@@ -6040,12 +6037,12 @@
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E27" s="19"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="J27" s="19"/>
       <c r="K27" s="3" t="s">
@@ -6073,16 +6070,16 @@
         <v>23</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="J28" s="19"/>
       <c r="K28" s="3"/>
@@ -6101,10 +6098,10 @@
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19" t="s">
@@ -6113,7 +6110,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J29" s="19"/>
       <c r="K29" s="3" t="s">
@@ -6135,14 +6132,14 @@
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J30" s="19"/>
       <c r="K30" s="3" t="s">
@@ -6170,12 +6167,12 @@
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J31" s="19"/>
       <c r="K31" s="3" t="s">
@@ -6197,14 +6194,14 @@
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
       <c r="I32" s="19" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J32" s="19"/>
       <c r="K32" s="3"/>
@@ -6225,11 +6222,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P8" sqref="P8"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C31" sqref="C31:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6519,7 +6516,7 @@
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>0</v>
@@ -6613,7 +6610,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9" t="s">
@@ -7285,7 +7282,9 @@
         <v>30</v>
       </c>
       <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="C31" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -7313,7 +7312,9 @@
         <v>31</v>
       </c>
       <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="C32" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D32" s="9" t="s">
         <v>129</v>
       </c>
@@ -7337,16 +7338,6 @@
         <v>8</v>
       </c>
       <c r="R32" s="3"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7359,9 +7350,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7420,8 +7411,8 @@
       <c r="N1" s="18">
         <v>35612</v>
       </c>
-      <c r="O1" s="18" t="s">
-        <v>257</v>
+      <c r="O1" s="18">
+        <v>35643</v>
       </c>
       <c r="P1" s="18">
         <v>35977</v>
@@ -7455,13 +7446,13 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -7473,7 +7464,7 @@
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -7483,11 +7474,11 @@
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="V2" s="3"/>
       <c r="W2" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -7499,7 +7490,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -7513,7 +7504,7 @@
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
@@ -7523,13 +7514,13 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -7539,17 +7530,17 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -7568,10 +7559,10 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -7581,17 +7572,17 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -7607,10 +7598,10 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W5" s="3"/>
     </row>
@@ -7623,15 +7614,15 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -7641,7 +7632,7 @@
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3" t="s">
@@ -7653,10 +7644,10 @@
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="W6" s="3"/>
     </row>
@@ -7671,19 +7662,19 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>176</v>
@@ -7693,7 +7684,7 @@
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3" t="s">
@@ -7705,13 +7696,13 @@
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -7725,25 +7716,25 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3" t="s">
@@ -7755,7 +7746,7 @@
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>250</v>
@@ -7773,19 +7764,19 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3" t="s">
@@ -7793,7 +7784,7 @@
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3" t="s">
@@ -7804,10 +7795,10 @@
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -7817,15 +7808,15 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -7849,10 +7840,10 @@
       </c>
       <c r="T10" s="3"/>
       <c r="U10" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="W10" s="3"/>
     </row>
@@ -7863,15 +7854,15 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
@@ -7879,7 +7870,7 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
@@ -7887,7 +7878,7 @@
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3" t="s">
@@ -7901,13 +7892,13 @@
       </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -7919,17 +7910,17 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
@@ -7937,7 +7928,7 @@
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>176</v>
@@ -7951,13 +7942,13 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -7973,7 +7964,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -7997,7 +7988,7 @@
       </c>
       <c r="T13" s="3"/>
       <c r="U13" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
@@ -8013,19 +8004,19 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3" t="s">
@@ -8033,7 +8024,7 @@
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3" t="s">
@@ -8045,7 +8036,7 @@
       </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
@@ -8059,15 +8050,15 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -8079,7 +8070,7 @@
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3" t="s">
@@ -8089,7 +8080,7 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
@@ -8105,27 +8096,27 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3" t="s">
@@ -8136,16 +8127,16 @@
         <v>221</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -8159,21 +8150,21 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
@@ -8181,7 +8172,7 @@
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3" t="s">
@@ -8192,16 +8183,16 @@
         <v>222</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="V17" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -8215,17 +8206,17 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3" t="s">
@@ -8243,11 +8234,11 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -8265,10 +8256,10 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -8283,7 +8274,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
@@ -8297,21 +8288,21 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3" t="s">
@@ -8331,11 +8322,11 @@
       </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="V20" s="3"/>
       <c r="W20" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -8351,17 +8342,17 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>181</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>226</v>
@@ -8384,10 +8375,10 @@
         <v>244</v>
       </c>
       <c r="V21" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -8403,15 +8394,15 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>227</v>
@@ -8430,7 +8421,7 @@
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W22" s="3"/>
     </row>
@@ -8445,17 +8436,17 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>228</v>
@@ -8479,7 +8470,7 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -8499,7 +8490,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>229</v>
@@ -8514,14 +8505,14 @@
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="V24" s="3"/>
       <c r="W24" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -8534,16 +8525,16 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3" t="s">
@@ -8563,7 +8554,7 @@
         <v>240</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -8583,7 +8574,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>230</v>
@@ -8603,10 +8594,10 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W26" s="3" t="s">
         <v>177</v>
@@ -8620,21 +8611,21 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
@@ -8652,7 +8643,7 @@
         <v>202</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W27" s="3"/>
     </row>
@@ -8666,13 +8657,13 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -8695,10 +8686,10 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="W28" s="3"/>
     </row>
@@ -8712,13 +8703,13 @@
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -8739,7 +8730,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
@@ -8754,7 +8745,7 @@
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
@@ -8762,7 +8753,7 @@
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="s">
@@ -8784,13 +8775,13 @@
       </c>
       <c r="S30" s="3"/>
       <c r="T30" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="U30" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="W30" s="3"/>
     </row>
@@ -8804,7 +8795,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
@@ -8812,7 +8803,7 @@
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -8837,10 +8828,10 @@
         <v>228</v>
       </c>
       <c r="U31" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="W31" s="3"/>
     </row>
@@ -8854,7 +8845,7 @@
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
@@ -8862,7 +8853,7 @@
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -8882,13 +8873,13 @@
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="U32" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W32" s="3"/>
     </row>
@@ -8903,9 +8894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK12" sqref="AK12"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9065,7 +9056,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -9073,52 +9064,52 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3" t="s">
         <v>225</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="X2" s="3"/>
       <c r="Y2" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>203</v>
       </c>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AD2" s="3"/>
       <c r="AE2" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -9132,7 +9123,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -9144,45 +9135,45 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="U3" s="3"/>
       <c r="V3" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="X3" s="3"/>
       <c r="Y3" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>187</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
@@ -9191,7 +9182,7 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>67</v>
@@ -9200,58 +9191,58 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>240</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="X4" s="3"/>
       <c r="Y4" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>210</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
       <c r="AI4" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AJ4" s="3"/>
     </row>
@@ -9261,7 +9252,7 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>35</v>
@@ -9271,7 +9262,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -9280,7 +9271,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
@@ -9290,39 +9281,39 @@
         <v>241</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="X5" s="3"/>
       <c r="Y5" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
       <c r="AI5" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -9332,48 +9323,48 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
@@ -9382,7 +9373,7 @@
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -9391,10 +9382,10 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -9403,7 +9394,7 @@
         <v>231</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -9412,26 +9403,26 @@
         <v>180</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
@@ -9445,12 +9436,12 @@
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -9459,44 +9450,44 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -9504,23 +9495,23 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -9529,43 +9520,43 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>133</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>206</v>
@@ -9573,30 +9564,30 @@
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
       <c r="AE9" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AF9" s="3"/>
       <c r="AG9" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -9609,58 +9600,58 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
         <v>234</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AF10" s="3"/>
       <c r="AG10" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -9669,61 +9660,61 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AJ11" s="3"/>
     </row>
@@ -9732,37 +9723,37 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -9779,26 +9770,26 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AG12" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -9808,32 +9799,32 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>235</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
@@ -9844,29 +9835,29 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3" t="s">
         <v>204</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -9876,7 +9867,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -9885,23 +9876,23 @@
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -9909,28 +9900,28 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -9945,60 +9936,60 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
         <v>236</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="X15" s="3"/>
       <c r="Y15" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
@@ -10009,49 +10000,49 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="X16" s="3"/>
       <c r="Y16" s="3" t="s">
@@ -10060,21 +10051,21 @@
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AC16" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AG16" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="AH16" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
@@ -10088,72 +10079,72 @@
         <v>193</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
       <c r="AF17" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AG17" s="3"/>
       <c r="AH17" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AI17" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="AJ17" s="3"/>
     </row>
@@ -10163,65 +10154,65 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="AH18" s="3"/>
       <c r="AI18" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AJ18" s="3"/>
     </row>
@@ -10230,20 +10221,20 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -10258,19 +10249,19 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
@@ -10278,10 +10269,10 @@
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
       <c r="AF19" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AG19" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
@@ -10292,24 +10283,24 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -10320,7 +10311,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
@@ -10330,7 +10321,7 @@
         <v>205</v>
       </c>
       <c r="X20" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
@@ -10338,16 +10329,16 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AH20" s="3"/>
       <c r="AI20" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AJ20" s="3"/>
     </row>
@@ -10357,23 +10348,23 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -10382,7 +10373,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -10392,26 +10383,26 @@
         <v>206</v>
       </c>
       <c r="X21" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AE21" s="3"/>
       <c r="AF21" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AG21" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
@@ -10423,28 +10414,28 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
@@ -10454,31 +10445,31 @@
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="W22" s="3"/>
       <c r="X22" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="Y22" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AE22" s="3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AH22" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AI22" s="3"/>
       <c r="AJ22" s="3"/>
@@ -10490,70 +10481,70 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>167</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="W23" s="3"/>
       <c r="X23" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AD23" s="3"/>
       <c r="AE23" s="3" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AF23" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AG23" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AH23" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="AI23" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="AJ23" s="3"/>
     </row>
@@ -10568,46 +10559,46 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="W24" s="3"/>
       <c r="X24" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AD24" s="3"/>
       <c r="AE24" s="3" t="s">
@@ -10615,10 +10606,10 @@
       </c>
       <c r="AF24" s="3"/>
       <c r="AG24" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AH24" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="3"/>
@@ -10629,71 +10620,71 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="Y25" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
       <c r="AB25" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AC25" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AD25" s="3"/>
       <c r="AE25" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AF25" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AG25" s="3"/>
       <c r="AH25" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AI25" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="AJ25" s="3"/>
     </row>
@@ -10704,7 +10695,7 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -10712,56 +10703,56 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>201</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="S26" s="3"/>
       <c r="T26" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="AC26" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
       <c r="AF26" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
       <c r="AI26" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AJ26" s="3"/>
     </row>
@@ -10782,11 +10773,11 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -10794,10 +10785,10 @@
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -10806,7 +10797,7 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
@@ -10815,7 +10806,7 @@
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
       <c r="AI27" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="AJ27" s="3"/>
     </row>
@@ -10825,24 +10816,24 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -10850,18 +10841,18 @@
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
@@ -10870,12 +10861,12 @@
       <c r="AD28" s="3"/>
       <c r="AE28" s="3"/>
       <c r="AF28" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
       <c r="AI28" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="AJ28" s="3"/>
     </row>
@@ -10890,41 +10881,41 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
       <c r="AB29" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
@@ -10933,7 +10924,7 @@
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AJ29" s="3"/>
     </row>
@@ -10946,42 +10937,42 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="W30" s="3"/>
       <c r="X30" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
@@ -10990,12 +10981,12 @@
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
       <c r="AF30" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AG30" s="3"/>
       <c r="AH30" s="3"/>
       <c r="AI30" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AJ30" s="3"/>
     </row>
@@ -11012,15 +11003,15 @@
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
@@ -11028,22 +11019,22 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="W31" s="3"/>
       <c r="X31" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Y31" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
@@ -11051,15 +11042,15 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AF31" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="AJ31" s="3"/>
     </row>
@@ -11079,7 +11070,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -11094,22 +11085,22 @@
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
       <c r="AB32" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>

</xml_diff>